<commit_message>
Added option to select certain rounds and Jg in ooebvrl Fixed bug in Spielerrangliste
</commit_message>
<xml_diff>
--- a/files/spielerranglisten/Spielerrangliste-2018-2019-alle.xlsx
+++ b/files/spielerranglisten/Spielerrangliste-2018-2019-alle.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>OÖBV - Mannschaftsmeisterschaft</t>
   </si>
@@ -29,10 +29,10 @@
     <t>S P I E L E R R A N G L I S T E</t>
   </si>
   <si>
-    <t>Stand per 09.01.2019</t>
-  </si>
-  <si>
-    <t>ABV  Wels</t>
+    <t>Stand per 22.01.2019</t>
+  </si>
+  <si>
+    <t>Österreichische Turn- und Sportunion Kirchdorf</t>
   </si>
   <si>
     <t>Änderungen/
@@ -66,37 +66,28 @@
     <t>1.</t>
   </si>
   <si>
-    <t>Tobias</t>
+    <t>Ofner</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
+    <t>Damen</t>
+  </si>
+  <si>
+    <t>Groiss</t>
+  </si>
+  <si>
+    <t>Emma</t>
   </si>
   <si>
     <t>2.</t>
   </si>
   <si>
-    <t>Hattinger</t>
-  </si>
-  <si>
-    <t>Die</t>
-  </si>
-  <si>
-    <t>MF</t>
-  </si>
-  <si>
-    <t>tobias.hattinger@gmx.at</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>Konkurenz</t>
-  </si>
-  <si>
-    <t>Halo</t>
-  </si>
-  <si>
-    <t>06605445095</t>
-  </si>
-  <si>
-    <t>Damen</t>
+    <t>Lungenschmied</t>
+  </si>
+  <si>
+    <t>Nora</t>
   </si>
 </sst>
 </file>
@@ -151,7 +142,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,12 +164,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -186,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -236,9 +221,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -575,10 +557,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,7 +661,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>6</v>
@@ -740,109 +722,73 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
-        <v>32323</v>
+      <c r="B12" t="s">
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
-        <v>3223</v>
+        <v>35694</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="3">
-        <v>442</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1">
+        <v>37933</v>
+      </c>
+      <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
-        <v>319</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="2" t="s">
+      <c r="F15" s="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1">
-        <v>5605</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D16" s="1">
+        <v>35614</v>
+      </c>
+      <c r="E16" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="1">
-        <v>319</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1">
-        <v>4433</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>319</v>
+      <c r="F16" s="1">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>